<commit_message>
delete baris jumlah total tiap kolom
</commit_message>
<xml_diff>
--- a/datasetdptdalamnegeripemilu2024_rev.xlsx
+++ b/datasetdptdalamnegeripemilu2024_rev.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wahib Muhibi Nur\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wahib Muhibi Nur\Documents\GitHub\dataset-finalassignment-add\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{427A7773-4EB3-4216-895F-F89F346767D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9240CF-078B-4801-8162-CAB45EAD65C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3165" yWindow="3840" windowWidth="21600" windowHeight="11295" xr2:uid="{5141B592-AB51-4EAA-9F75-61453BB73D01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="559">
   <si>
     <t>Nama Provinsi</t>
   </si>
@@ -1698,9 +1698,6 @@
   </si>
   <si>
     <t>KOTA SORONG</t>
-  </si>
-  <si>
-    <t>JUMLAH TOTAL</t>
   </si>
   <si>
     <t>Jumlah Kelurahan/Desa</t>
@@ -1816,7 +1813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="41" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1827,9 +1824,6 @@
     <xf numFmtId="41" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1838,9 +1832,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2157,10 +2148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113DA957-780C-403D-A647-E37D8DBC681A}">
-  <dimension ref="A1:H516"/>
+  <dimension ref="A1:H515"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A494" workbookViewId="0">
+      <selection activeCell="B509" sqref="B509"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,29 +2166,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>555</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>558</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>559</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>557</v>
+      <c r="H1" s="5" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12033,7 +12024,7 @@
         <v>398</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C380" s="2">
         <v>10</v>
@@ -15564,40 +15555,7 @@
         <v>205507</v>
       </c>
     </row>
-    <row r="516" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A516" s="8" t="s">
-        <v>554</v>
-      </c>
-      <c r="B516" s="8"/>
-      <c r="C516" s="4">
-        <f>SUM(C2:C515)</f>
-        <v>7277</v>
-      </c>
-      <c r="D516" s="4">
-        <f t="shared" ref="D516:H516" si="0">SUM(D2:D515)</f>
-        <v>83731</v>
-      </c>
-      <c r="E516" s="4">
-        <f t="shared" si="0"/>
-        <v>820161</v>
-      </c>
-      <c r="F516" s="4">
-        <f t="shared" si="0"/>
-        <v>101467243</v>
-      </c>
-      <c r="G516" s="4">
-        <f t="shared" si="0"/>
-        <v>101589505</v>
-      </c>
-      <c r="H516" s="4">
-        <f t="shared" si="0"/>
-        <v>203056748</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A516:B516"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>